<commit_message>
updated api for bdd
</commit_message>
<xml_diff>
--- a/getDataFromExcel.xlsx
+++ b/getDataFromExcel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse-Workplace\DockerAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AE7C04-264A-4131-8242-2FB94E00E0DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B48CFD3-96FC-4C2D-AAFD-E42EF3D126A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RestAssured" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateUser" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Rest</t>
   </si>
@@ -76,16 +77,48 @@
   </si>
   <si>
     <t>343434</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>vipin</t>
+  </si>
+  <si>
+    <t>v@v.com</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,14 +141,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -396,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,4 +523,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4E4BF9-0301-4798-A73E-423A0DA93CF1}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{71A24621-B873-4220-A8F6-62BF4A63EF66}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>